<commit_message>
Latest migration config from Andrea. Fixed a couple of issues in the code and in the data.
</commit_message>
<xml_diff>
--- a/Migration_Data.xlsx
+++ b/Migration_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7900" yWindow="5600" windowWidth="27760" windowHeight="15540" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="38400" yWindow="-7360" windowWidth="21600" windowHeight="37940" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="756">
   <si>
     <t>Source</t>
   </si>
@@ -2315,6 +2315,30 @@
   </si>
   <si>
     <t>contained</t>
+  </si>
+  <si>
+    <t>SP6</t>
+  </si>
+  <si>
+    <t>SP5</t>
+  </si>
+  <si>
+    <t>Geometric Place Expression?</t>
+  </si>
+  <si>
+    <t>Declarative Place?</t>
+  </si>
+  <si>
+    <t>SP4</t>
+  </si>
+  <si>
+    <t>Spatial coordinates reference system?</t>
+  </si>
+  <si>
+    <t>E100</t>
+  </si>
+  <si>
+    <t>Recommendation Plan?</t>
   </si>
 </sst>
 </file>
@@ -3406,10 +3430,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C93"/>
+  <dimension ref="A1:C115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3448,7 +3472,7 @@
         <v>57</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C7" si="0">CONCATENATE("INSERT INTO ontology.classes VALUES('", A3, "', '", B3, "', true);")</f>
+        <f t="shared" ref="C3:C11" si="0">CONCATENATE("INSERT INTO ontology.classes VALUES('", A3, "', '", B3, "', true);")</f>
         <v>INSERT INTO ontology.classes VALUES('I6', 'Archaeology Certainty Value', true);</v>
       </c>
     </row>
@@ -3501,690 +3525,738 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>311</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>639</v>
+      <c r="A8" t="s">
+        <v>748</v>
+      </c>
+      <c r="B8" t="s">
+        <v>751</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ontology.classes VALUES('SP6', 'Declarative Place?', true);</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>640</v>
+      <c r="A9" t="s">
+        <v>749</v>
+      </c>
+      <c r="B9" t="s">
+        <v>750</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ontology.classes VALUES('SP5', 'Geometric Place Expression?', true);</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>363</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>641</v>
+      <c r="A10" t="s">
+        <v>752</v>
+      </c>
+      <c r="B10" t="s">
+        <v>753</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ontology.classes VALUES('SP4', 'Spatial coordinates reference system?', true);</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>644</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>646</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>649</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>410</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>500</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>445</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>656</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>658</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>416</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
-        <v>456</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>444</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
-        <v>663</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
-        <v>469</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>666</v>
+      <c r="A11" t="s">
+        <v>754</v>
+      </c>
+      <c r="B11" t="s">
+        <v>755</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ontology.classes VALUES('E100', 'Recommendation Plan?', true);</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>493</v>
+        <v>311</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>667</v>
+        <v>639</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>496</v>
+        <v>190</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>668</v>
+        <v>640</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>504</v>
+        <v>363</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>669</v>
+        <v>641</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>518</v>
+        <v>81</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>670</v>
+        <v>642</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>97</v>
+        <v>151</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>671</v>
+        <v>643</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>100</v>
+        <v>644</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>672</v>
+        <v>645</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>108</v>
+        <v>646</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>673</v>
+        <v>647</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>198</v>
+        <v>71</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>674</v>
+        <v>648</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>675</v>
+        <v>649</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>676</v>
+        <v>650</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>168</v>
+        <v>410</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>677</v>
+        <v>651</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>128</v>
+        <v>500</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>678</v>
+        <v>652</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>136</v>
+        <v>445</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>679</v>
+        <v>653</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>294</v>
+        <v>101</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>680</v>
+        <v>654</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>144</v>
+        <v>233</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>681</v>
+        <v>655</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>180</v>
+        <v>656</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>682</v>
+        <v>657</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
-        <v>222</v>
+        <v>658</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>683</v>
+        <v>659</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
-        <v>684</v>
+        <v>416</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>685</v>
+        <v>660</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
-        <v>253</v>
+        <v>456</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>686</v>
+        <v>661</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
-        <v>260</v>
+        <v>444</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>687</v>
+        <v>662</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
-        <v>267</v>
+        <v>663</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>688</v>
+        <v>664</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>689</v>
+        <v>665</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
-        <v>82</v>
+        <v>469</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>690</v>
+        <v>666</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
-        <v>117</v>
+        <v>493</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>691</v>
+        <v>667</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
-        <v>202</v>
+        <v>496</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>692</v>
+        <v>668</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
-        <v>125</v>
+        <v>504</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>693</v>
+        <v>669</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
-        <v>243</v>
+        <v>518</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>694</v>
+        <v>670</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
-        <v>348</v>
+        <v>97</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>695</v>
+        <v>671</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>696</v>
+        <v>672</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
-        <v>373</v>
+        <v>108</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>697</v>
+        <v>673</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
-        <v>141</v>
+        <v>198</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>698</v>
+        <v>674</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
-        <v>91</v>
+        <v>675</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>699</v>
+        <v>676</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
-        <v>700</v>
+        <v>168</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>701</v>
+        <v>677</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
-        <v>320</v>
+        <v>128</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>702</v>
+        <v>678</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
-        <v>353</v>
+        <v>136</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>703</v>
+        <v>679</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
-        <v>109</v>
+        <v>294</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>704</v>
+        <v>680</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
-        <v>435</v>
+        <v>144</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>705</v>
+        <v>681</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
-        <v>439</v>
+        <v>180</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>706</v>
+        <v>682</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
-        <v>707</v>
+        <v>222</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>708</v>
+        <v>683</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
-        <v>709</v>
+        <v>684</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>710</v>
+        <v>685</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
-        <v>114</v>
+        <v>253</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>711</v>
+        <v>686</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
-        <v>85</v>
+        <v>260</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>712</v>
+        <v>687</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
-        <v>236</v>
+        <v>267</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>713</v>
+        <v>688</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
-        <v>356</v>
+        <v>201</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>714</v>
+        <v>689</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
-        <v>479</v>
+        <v>82</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>715</v>
+        <v>690</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
-        <v>716</v>
+        <v>117</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>717</v>
+        <v>691</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
-        <v>718</v>
+        <v>202</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>719</v>
+        <v>692</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
-        <v>720</v>
+        <v>125</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>721</v>
+        <v>693</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
-        <v>459</v>
+        <v>243</v>
       </c>
       <c r="B77" s="5" t="s">
-        <v>722</v>
+        <v>694</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
-        <v>131</v>
+        <v>348</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>723</v>
+        <v>695</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
-        <v>724</v>
+        <v>250</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>725</v>
+        <v>696</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>726</v>
+        <v>697</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>727</v>
+        <v>698</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
-        <v>322</v>
+        <v>91</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>728</v>
+        <v>699</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
-        <v>96</v>
+        <v>700</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>2</v>
+        <v>701</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
-        <v>191</v>
+        <v>320</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>729</v>
+        <v>702</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
-        <v>488</v>
+        <v>353</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>730</v>
+        <v>703</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
-        <v>413</v>
+        <v>109</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>731</v>
+        <v>704</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
-        <v>462</v>
+        <v>435</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>732</v>
+        <v>705</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="5" t="s">
-        <v>499</v>
+        <v>439</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>733</v>
+        <v>706</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
-        <v>509</v>
+        <v>707</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>734</v>
+        <v>708</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="5" t="s">
-        <v>90</v>
+        <v>709</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>735</v>
+        <v>710</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="5" t="s">
-        <v>187</v>
+        <v>114</v>
       </c>
       <c r="B91" s="5" t="s">
-        <v>736</v>
+        <v>711</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
-        <v>122</v>
+        <v>85</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>737</v>
+        <v>712</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="5" t="s">
+        <v>716</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="5" t="s">
+        <v>718</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="5" t="s">
+        <v>720</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="5" t="s">
+        <v>724</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="5" t="s">
+        <v>462</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="5" t="s">
+        <v>499</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="B93" s="5" t="s">
+      <c r="B115" s="5" t="s">
         <v>738</v>
       </c>
     </row>
@@ -8009,8 +8081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>